<commit_message>
edited functions to be better
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b756f5c37f55a3ba/Documents/R_Projects/Keller Research Team/waterresourcerers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EADD55A-02FF-4871-AF1F-46167B9D4C99}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F7B361E-196A-428E-8464-FD1E57F87CFE}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="13320" windowHeight="11295" xr2:uid="{0F7B361E-196A-428E-8464-FD1E57F87CFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>groundwater recharge</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>nanofiltration</t>
   </si>
 </sst>
 </file>
@@ -145,6 +151,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C06CD0-7E55-44BC-931B-A9C8313A4E18}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +465,7 @@
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,8 +490,11 @@
       <c r="H1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -506,8 +519,11 @@
       <c r="H2">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -533,8 +549,11 @@
         <f>AVERAGE(0.07, 0.1, 0.2)</f>
         <v>0.12333333333333334</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -559,8 +578,11 @@
       <c r="H4">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -580,8 +602,11 @@
         <f>AVERAGE(0.05*3.79,0.12*3.79)/24</f>
         <v>1.3422916666666666E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -601,8 +626,11 @@
         <f>AVERAGE(0.01, 0.05)</f>
         <v>3.0000000000000002E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -622,61 +650,102 @@
         <f>0.18/24</f>
         <v>7.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <v>0.74</v>
-      </c>
-      <c r="C8">
-        <v>3.95</v>
-      </c>
       <c r="H8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.81</v>
+        <v>9.3422999999999998</v>
       </c>
       <c r="C9">
-        <v>4.07</v>
+        <v>0.7177</v>
       </c>
       <c r="E9">
-        <v>9.0527999999999995</v>
+        <v>2.9129</v>
       </c>
       <c r="F9">
-        <v>-20.495000000000001</v>
+        <v>0.64839999999999998</v>
       </c>
       <c r="H9">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
+      </c>
+      <c r="B11">
+        <v>0.222</v>
+      </c>
+      <c r="C11">
+        <v>1.516</v>
+      </c>
+      <c r="D11">
+        <v>3.0710000000000002</v>
+      </c>
+      <c r="E11">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="F11">
+        <v>1.448</v>
+      </c>
+      <c r="G11">
+        <v>2.726</v>
       </c>
       <c r="H11">
         <f>AVERAGE(0.4, 0.7)</f>
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="H12">
         <v>0.48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>7.14</v>
+      </c>
+      <c r="C13">
+        <v>-0.22</v>
+      </c>
+      <c r="E13">
+        <v>0.44</v>
+      </c>
+      <c r="F13">
+        <v>-0.13</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more linear models
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b756f5c37f55a3ba/Documents/R_Projects/Keller Research Team/waterresourcerers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46FD3BA4-7411-47F3-BCAD-7E29AE7D8FD5}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F19E22D-D704-4845-AA12-F7620824EBA2}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="3975" windowWidth="13320" windowHeight="11295" xr2:uid="{0F7B361E-196A-428E-8464-FD1E57F87CFE}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{0F7B361E-196A-428E-8464-FD1E57F87CFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>nanofiltration</t>
+  </si>
+  <si>
+    <t>water loss</t>
+  </si>
+  <si>
+    <t>drinking water treatment</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C06CD0-7E55-44BC-931B-A9C8313A4E18}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,6 +768,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added error to the energy
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b756f5c37f55a3ba/Documents/R_Projects/Keller Research Team/waterresourcerers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F19E22D-D704-4845-AA12-F7620824EBA2}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48182AA6-E9F0-4D2F-A5B7-9D3F35AF2DB3}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{0F7B361E-196A-428E-8464-FD1E57F87CFE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F7B361E-196A-428E-8464-FD1E57F87CFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -101,10 +101,7 @@
     <t>nanofiltration</t>
   </si>
   <si>
-    <t>water loss</t>
-  </si>
-  <si>
-    <t>drinking water treatment</t>
+    <t>var</t>
   </si>
 </sst>
 </file>
@@ -452,7 +449,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -460,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C06CD0-7E55-44BC-931B-A9C8313A4E18}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +468,7 @@
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,10 +494,13 @@
         <v>16</v>
       </c>
       <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -523,13 +523,18 @@
         <v>2.786</v>
       </c>
       <c r="H2">
-        <v>0.54</v>
+        <f>AVERAGE(1, 2.5)</f>
+        <v>1.75</v>
       </c>
       <c r="I2">
+        <f>_xlfn.VAR.P(1,2.5)</f>
+        <v>0.5625</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -552,14 +557,18 @@
         <v>1.8759999999999999</v>
       </c>
       <c r="H3">
-        <f>AVERAGE(0.07, 0.1, 0.2)</f>
-        <v>0.12333333333333334</v>
+        <f>AVERAGE(0.13, 0.177, 0.201, 0.2, 0.3)</f>
+        <v>0.2016</v>
       </c>
       <c r="I3">
+        <f>_xlfn.VAR.P(0.07, 0.1, 0.2)</f>
+        <v>3.0888888888888941E-3</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -584,11 +593,11 @@
       <c r="H4">
         <v>0.37</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -609,10 +618,14 @@
         <v>1.3422916666666666E-2</v>
       </c>
       <c r="I5">
+        <f>_xlfn.VAR.P(0.05*3.79,0.12*3.79)/24</f>
+        <v>7.3316760416666674E-4</v>
+      </c>
+      <c r="J5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -629,14 +642,18 @@
         <v>-5.1999999999999998E-2</v>
       </c>
       <c r="H6">
-        <f>AVERAGE(0.01, 0.05)</f>
-        <v>3.0000000000000002E-2</v>
+        <f>AVERAGE(36.46, 36.46, 35.61, 36.64, 36.91, 35.43) / 1000</f>
+        <v>3.6251666666666675E-2</v>
       </c>
       <c r="I6">
+        <f>_xlfn.VAR.P(36.46, 36.46, 35.61, 36.64, 36.91, 35.43) / 1000</f>
+        <v>2.929805555555552E-4</v>
+      </c>
+      <c r="J6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -653,13 +670,18 @@
         <v>-0.22</v>
       </c>
       <c r="H7">
-        <v>0.18</v>
+        <f>AVERAGE(0.11, 0.24, 0.2, 0.2, 0.3)</f>
+        <v>0.21000000000000002</v>
       </c>
       <c r="I7">
+        <f>_xlfn.VAR.P(0.11, 0.24, 0.2, 0.2, 0.3)</f>
+        <v>3.8399999999999945E-3</v>
+      </c>
+      <c r="J7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -676,13 +698,18 @@
         <v>330.13</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <f>AVERAGE(1.02, 2.57)</f>
+        <v>1.7949999999999999</v>
       </c>
       <c r="I8">
+        <f>_xlfn.VAR.P(1.02, 2.57)</f>
+        <v>0.60062499999999952</v>
+      </c>
+      <c r="J8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -699,18 +726,23 @@
         <v>0.64839999999999998</v>
       </c>
       <c r="H9">
-        <v>3.8</v>
+        <f>AVERAGE(2.58,5.47)</f>
+        <v>4.0250000000000004</v>
       </c>
       <c r="I9">
+        <f>_xlfn.VAR.P(2.58,5.47)</f>
+        <v>2.0880249999999947</v>
+      </c>
+      <c r="J9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -737,10 +769,14 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="I11">
+        <f>_xlfn.VAR.P(0.4, 0.7)</f>
+        <v>2.2499999999999909E-2</v>
+      </c>
+      <c r="J11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -748,7 +784,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -764,18 +800,16 @@
       <c r="F13">
         <v>-0.13</v>
       </c>
+      <c r="H13">
+        <f>AVERAGE(1.33, 0.68, 1.17)</f>
+        <v>1.06</v>
+      </c>
       <c r="I13">
+        <f>_xlfn.VAR.P(1.33, 0.68, 1.17)</f>
+        <v>7.6466666666666488E-2</v>
+      </c>
+      <c r="J13">
         <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited data and functions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b756f5c37f55a3ba/Documents/R_Projects/Keller Research Team/waterresourcerers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48182AA6-E9F0-4D2F-A5B7-9D3F35AF2DB3}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06DC76CD-7E39-4231-AD08-D17AA1A66778}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F7B361E-196A-428E-8464-FD1E57F87CFE}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{0F7B361E-196A-428E-8464-FD1E57F87CFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
error output in table
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b756f5c37f55a3ba/Documents/R_Projects/Keller Research Team/waterresourcerers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06DC76CD-7E39-4231-AD08-D17AA1A66778}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C9D9C9B-B2CD-4565-8C5F-D2608087EB76}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{0F7B361E-196A-428E-8464-FD1E57F87CFE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>coagulation</t>
-  </si>
-  <si>
-    <t>groundwater recharge</t>
   </si>
   <si>
     <t>model</t>
@@ -457,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C06CD0-7E55-44BC-931B-A9C8313A4E18}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,10 +491,10 @@
         <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -778,37 +775,29 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>7.14</v>
+      </c>
+      <c r="C12">
+        <v>-0.22</v>
+      </c>
+      <c r="E12">
+        <v>0.44</v>
+      </c>
+      <c r="F12">
+        <v>-0.13</v>
       </c>
       <c r="H12">
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>7.14</v>
-      </c>
-      <c r="C13">
-        <v>-0.22</v>
-      </c>
-      <c r="E13">
-        <v>0.44</v>
-      </c>
-      <c r="F13">
-        <v>-0.13</v>
-      </c>
-      <c r="H13">
         <f>AVERAGE(1.33, 0.68, 1.17)</f>
         <v>1.06</v>
       </c>
-      <c r="I13">
+      <c r="I12">
         <f>_xlfn.VAR.P(1.33, 0.68, 1.17)</f>
         <v>7.6466666666666488E-2</v>
       </c>
-      <c r="J13">
+      <c r="J12">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ADDING GROUNWATER PUMPING O&m
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b756f5c37f55a3ba/Documents/R_Projects/Keller Research Team/waterresourcerers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2461F40F-B6FD-49C6-B3DD-27E4BC41196E}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="8_{D53394B7-E1C1-4D24-B1E4-489381E175AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E463FE9F-203C-4341-9515-DE5FBACB415E}"/>
   <bookViews>
     <workbookView xWindow="-11990" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{0F7B361E-196A-428E-8464-FD1E57F87CFE}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +765,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>